<commit_message>
learning openpyxl python library
learning openpyxl python library
</commit_message>
<xml_diff>
--- a/PYTHON AUTOMATION/excel.xlsx
+++ b/PYTHON AUTOMATION/excel.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="firstsheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Secondsheet" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,6 +414,52 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Total_sales</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>40000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>